<commit_message>
Updated BOM for CPU sheet.
</commit_message>
<xml_diff>
--- a/RavAGE-0.1-alpha-RC1-BOM.xlsx
+++ b/RavAGE-0.1-alpha-RC1-BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
   <si>
     <t>RavAGE 0.1-alpha</t>
   </si>
@@ -120,12 +120,6 @@
     <t>MC9S12XDP512MAG</t>
   </si>
   <si>
-    <t>M41T56M6</t>
-  </si>
-  <si>
-    <t>IC, RTC</t>
-  </si>
-  <si>
     <t>IC, MICROCONTROLLER, FREESCALE</t>
   </si>
   <si>
@@ -192,12 +186,6 @@
     <t>MCCA000255</t>
   </si>
   <si>
-    <t>10uF Capacitor Tantalum 10V 20% 0805</t>
-  </si>
-  <si>
-    <t>TPSP106M010R2000</t>
-  </si>
-  <si>
     <t>ABRACON</t>
   </si>
   <si>
@@ -214,6 +202,27 @@
   </si>
   <si>
     <t>HCM49 16.000MABJ-UT</t>
+  </si>
+  <si>
+    <t>JOHANSON DIELECTRICS</t>
+  </si>
+  <si>
+    <t>10uF Capacitor MLCC 10V 10% 0805 (min order qty of 10)</t>
+  </si>
+  <si>
+    <t>100R15X106KV4E</t>
+  </si>
+  <si>
+    <t>FREESCALE</t>
+  </si>
+  <si>
+    <t>M41T56M6E</t>
+  </si>
+  <si>
+    <t>IC, RTCC</t>
+  </si>
+  <si>
+    <t>STMICROELECTRONICS</t>
   </si>
 </sst>
 </file>
@@ -221,7 +230,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.000"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -300,29 +309,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,7 +639,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,7 +647,7 @@
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -646,478 +655,494 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="5">
         <v>9238549</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="5">
         <v>50</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="6">
         <f>F5*G5</f>
         <v>0.4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="5">
         <v>9238603</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="5">
         <v>50</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="6">
         <f>F6*G6</f>
         <v>0.4</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="5">
         <v>1469766</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="5">
         <v>1</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="6">
         <v>0.05</v>
       </c>
-      <c r="H7" s="9">
-        <f t="shared" ref="H7:H31" si="0">F7*G7</f>
+      <c r="H7" s="6">
+        <f t="shared" ref="H7:H21" si="0">F7*G7</f>
         <v>0.05</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="5">
         <v>9238484</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="5">
         <v>50</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="6">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="E9" s="5">
+        <v>1327683</v>
+      </c>
+      <c r="F9" s="5">
+        <v>10</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.106</v>
+      </c>
+      <c r="H9" s="6">
+        <f t="shared" si="0"/>
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="C10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="8">
-        <v>1327683</v>
-      </c>
-      <c r="F9" s="8">
+      <c r="D10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1414620</v>
+      </c>
+      <c r="F10" s="5">
         <v>10</v>
       </c>
-      <c r="G9" s="9">
-        <v>0.106</v>
-      </c>
-      <c r="H9" s="9">
-        <f t="shared" si="0"/>
-        <v>1.06</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="8" t="s">
+      <c r="G10" s="6">
+        <v>2.4E-2</v>
+      </c>
+      <c r="H10" s="6">
+        <f t="shared" si="0"/>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="8">
-        <v>1414620</v>
-      </c>
-      <c r="F10" s="8">
+      <c r="E11" s="5">
+        <v>1414649</v>
+      </c>
+      <c r="F11" s="5">
         <v>10</v>
       </c>
-      <c r="G10" s="9">
-        <v>2.4E-2</v>
-      </c>
-      <c r="H10" s="9">
-        <f t="shared" si="0"/>
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="8" t="s">
+      <c r="G11" s="6">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="H11" s="6">
+        <f t="shared" si="0"/>
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="8">
-        <v>1414649</v>
-      </c>
-      <c r="F11" s="8">
+      <c r="D12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="5">
+        <v>1813442</v>
+      </c>
+      <c r="F12" s="5">
         <v>10</v>
       </c>
-      <c r="G11" s="9">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="H11" s="9">
-        <f t="shared" si="0"/>
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="8" t="s">
+      <c r="G12" s="6">
+        <v>0.114</v>
+      </c>
+      <c r="H12" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1400000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="8">
-        <v>1813442</v>
-      </c>
-      <c r="F12" s="8">
+      <c r="E13" s="5">
+        <v>1759122</v>
+      </c>
+      <c r="F13" s="5">
+        <v>100</v>
+      </c>
+      <c r="G13" s="6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="H13" s="6">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="5">
+        <v>1886102</v>
+      </c>
+      <c r="F14" s="5">
         <v>10</v>
       </c>
-      <c r="G12" s="9">
-        <v>0.114</v>
-      </c>
-      <c r="H12" s="9">
-        <f t="shared" si="0"/>
-        <v>1.1400000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="8" t="s">
+      <c r="G14" s="6">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="H14" s="6">
+        <f t="shared" si="0"/>
+        <v>2.58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="5">
+        <v>1611734</v>
+      </c>
+      <c r="F18" s="5">
+        <v>1</v>
+      </c>
+      <c r="G18" s="6">
+        <v>1.2</v>
+      </c>
+      <c r="H18" s="6">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="D19" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="8">
-        <v>1759122</v>
-      </c>
-      <c r="F13" s="8">
-        <v>100</v>
-      </c>
-      <c r="G13" s="9">
-        <v>1.6E-2</v>
-      </c>
-      <c r="H13" s="9">
-        <f t="shared" si="0"/>
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="8">
-        <v>1658716</v>
-      </c>
-      <c r="F14" s="8">
-        <v>4</v>
-      </c>
-      <c r="G14" s="9">
-        <v>0.73399999999999999</v>
-      </c>
-      <c r="H14" s="9">
-        <f t="shared" si="0"/>
-        <v>2.9359999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="8" t="s">
+      <c r="E19" s="5">
+        <v>1633675</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1</v>
+      </c>
+      <c r="G19" s="6">
+        <v>1.8</v>
+      </c>
+      <c r="H19" s="6">
+        <f t="shared" si="0"/>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18" s="8">
-        <v>1611734</v>
-      </c>
-      <c r="F18" s="8">
+      <c r="E20" s="5">
+        <v>1579847</v>
+      </c>
+      <c r="F20" s="5">
         <v>1</v>
       </c>
-      <c r="G18" s="9">
-        <v>1.2</v>
-      </c>
-      <c r="H18" s="9">
-        <f t="shared" si="0"/>
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" s="8">
-        <v>1633675</v>
-      </c>
-      <c r="F19" s="8">
+      <c r="G20" s="6">
+        <v>39.24</v>
+      </c>
+      <c r="H20" s="6">
+        <f t="shared" si="0"/>
+        <v>39.24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="5">
+        <v>9882650</v>
+      </c>
+      <c r="F21" s="5">
         <v>1</v>
       </c>
-      <c r="G19" s="9">
-        <v>1.8</v>
-      </c>
-      <c r="H19" s="9">
-        <f t="shared" si="0"/>
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="G21" s="6">
+        <v>2.4</v>
+      </c>
+      <c r="H21" s="6">
+        <f t="shared" si="0"/>
+        <v>2.4</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated BOM to contain USB Comms and RS232 Comms component information.
</commit_message>
<xml_diff>
--- a/RavAGE-0.1-alpha-RC1-BOM.xlsx
+++ b/RavAGE-0.1-alpha-RC1-BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="196">
   <si>
     <t>RavAGE 0.1-alpha</t>
   </si>
@@ -130,9 +130,6 @@
     <t>BDM Header 2x3 DIL</t>
   </si>
   <si>
-    <t>Firmware Load Jumper 1x2 SIL</t>
-  </si>
-  <si>
     <t>0603ZC224KAT2A</t>
   </si>
   <si>
@@ -458,6 +455,153 @@
   </si>
   <si>
     <t>IC, RTCC, SOIC-8</t>
+  </si>
+  <si>
+    <t>USB Comms.SchDoc</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>R18, R19, R20</t>
+  </si>
+  <si>
+    <t>2k Resistor 100mW 1% 0603</t>
+  </si>
+  <si>
+    <t>***refer to R8 on CPU.SchDoc page of BOM***</t>
+  </si>
+  <si>
+    <t>2073418 (min order qty of 100)</t>
+  </si>
+  <si>
+    <t>MCMR06X2001FTL</t>
+  </si>
+  <si>
+    <t>C26</t>
+  </si>
+  <si>
+    <t>C27, C29</t>
+  </si>
+  <si>
+    <t>C28</t>
+  </si>
+  <si>
+    <t>4.7uF Capacitor MLCC 10V 10% 0603</t>
+  </si>
+  <si>
+    <t>1833806 (min order qty of 10)</t>
+  </si>
+  <si>
+    <t>0603ZD475KAT2A</t>
+  </si>
+  <si>
+    <t>10nF Capacitor X7R Ceramic 50V 10% 0603</t>
+  </si>
+  <si>
+    <t>1833842 (min order qty of 5)</t>
+  </si>
+  <si>
+    <t>06035C103K4Z2A</t>
+  </si>
+  <si>
+    <t>FB1</t>
+  </si>
+  <si>
+    <t>1515741 (min order qty of 5)</t>
+  </si>
+  <si>
+    <t>MURATA</t>
+  </si>
+  <si>
+    <t>BLM18PG300SN1D</t>
+  </si>
+  <si>
+    <t>FERRITE BEAD, 0.05R, 1A, 0603</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>USB</t>
+  </si>
+  <si>
+    <t>FT232RL</t>
+  </si>
+  <si>
+    <t>FTDI</t>
+  </si>
+  <si>
+    <t>ANALOG DEVICES</t>
+  </si>
+  <si>
+    <t>ISOLATOR, DIGITAL, 150NS, SOIC-8</t>
+  </si>
+  <si>
+    <t>ADUM3201ARZ</t>
+  </si>
+  <si>
+    <t>IC, USB TO UART, SSOP-28</t>
+  </si>
+  <si>
+    <t>MOLEX</t>
+  </si>
+  <si>
+    <t>51387-0578</t>
+  </si>
+  <si>
+    <t>MINI USB TYPE B, RECEPTACLE</t>
+  </si>
+  <si>
+    <t>CBUSIO</t>
+  </si>
+  <si>
+    <t>TXLED, RXLED, CBUS3LED</t>
+  </si>
+  <si>
+    <t>Header 1x2 SIL</t>
+  </si>
+  <si>
+    <t>Firmware Load Jumper, Header 1x2 SIL</t>
+  </si>
+  <si>
+    <t>RS232 Comms.SchDoc</t>
+  </si>
+  <si>
+    <t>C30, C31, C32, C33, C34</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>JP2</t>
+  </si>
+  <si>
+    <t>MAX232ACWE</t>
+  </si>
+  <si>
+    <t>IC, TRANSCEIVER, SOIC-16</t>
+  </si>
+  <si>
+    <t>MAXIM</t>
+  </si>
+  <si>
+    <t>SCHURTER</t>
+  </si>
+  <si>
+    <t>152204 (min order qty of 2)</t>
+  </si>
+  <si>
+    <t>SOCKET, 3.5MM, JACK, PCB, 3POLE</t>
+  </si>
+  <si>
+    <t>VR Interfaces.SchDoc</t>
   </si>
 </sst>
 </file>
@@ -532,7 +676,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -555,20 +699,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -598,18 +733,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -622,6 +745,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -926,10 +1050,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,40 +1069,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1011,7 +1135,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>16</v>
@@ -1020,7 +1144,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F5" s="2">
         <v>50</v>
@@ -1038,7 +1162,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>17</v>
@@ -1047,7 +1171,7 @@
         <v>15</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F6" s="2">
         <v>50</v>
@@ -1092,7 +1216,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>21</v>
@@ -1101,7 +1225,7 @@
         <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F8" s="2">
         <v>50</v>
@@ -1119,16 +1243,16 @@
         <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F9" s="2">
         <v>10</v>
@@ -1146,16 +1270,16 @@
         <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F10" s="2">
         <v>10</v>
@@ -1173,16 +1297,16 @@
         <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F11" s="2">
         <v>10</v>
@@ -1200,16 +1324,16 @@
         <v>24</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F12" s="2">
         <v>10</v>
@@ -1227,16 +1351,16 @@
         <v>27</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F13" s="2">
         <v>100</v>
@@ -1254,16 +1378,16 @@
         <v>26</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F14" s="2">
         <v>10</v>
@@ -1315,7 +1439,7 @@
         <v>36</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>38</v>
+        <v>183</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="2"/>
@@ -1332,13 +1456,13 @@
         <v>32</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="E18" s="2">
         <v>1611734</v>
@@ -1359,13 +1483,13 @@
         <v>33</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="D19" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" s="2">
         <v>1633675</v>
@@ -1386,13 +1510,13 @@
         <v>28</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E20" s="2">
         <v>1579847</v>
@@ -1413,13 +1537,13 @@
         <v>29</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="E21" s="2">
         <v>9882650</v>
@@ -1436,40 +1560,40 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A22" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
+      <c r="A22" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
     </row>
     <row r="23" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A24" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
+      <c r="A24" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
     </row>
     <row r="25" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
@@ -1499,19 +1623,19 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="F26" s="2">
         <v>50</v>
@@ -1526,19 +1650,19 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="F27" s="2">
         <v>5</v>
@@ -1553,19 +1677,19 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F28" s="2">
         <v>5</v>
@@ -1580,19 +1704,19 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F29" s="2">
         <v>50</v>
@@ -1607,16 +1731,16 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E30" s="10">
         <v>1653317</v>
@@ -1634,16 +1758,16 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E31" s="2">
         <v>1752458</v>
@@ -1661,16 +1785,16 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="10" t="s">
         <v>89</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>90</v>
       </c>
       <c r="E32" s="10">
         <v>2100124</v>
@@ -1688,19 +1812,19 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="F33" s="2">
         <v>10</v>
@@ -1715,19 +1839,19 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="F34" s="2">
         <v>10</v>
@@ -1742,16 +1866,16 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
+        <v>85</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
       <c r="F35" s="8">
         <v>0</v>
       </c>
@@ -1765,24 +1889,24 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="F36" s="2">
         <v>10</v>
       </c>
-      <c r="G36" s="2">
+      <c r="G36" s="3">
         <v>0.376</v>
       </c>
       <c r="H36" s="3">
@@ -1792,24 +1916,24 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="F37" s="2">
         <v>10</v>
       </c>
-      <c r="G37" s="2">
+      <c r="G37" s="3">
         <v>1.82</v>
       </c>
       <c r="H37" s="3">
@@ -1819,7 +1943,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>34</v>
@@ -1828,7 +1952,7 @@
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
+      <c r="G38" s="15"/>
       <c r="H38" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1836,24 +1960,24 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>144</v>
       </c>
       <c r="F39" s="2">
         <v>10</v>
       </c>
-      <c r="G39" s="2">
+      <c r="G39" s="3">
         <v>1.1399999999999999</v>
       </c>
       <c r="H39" s="3">
@@ -1863,16 +1987,16 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="E40" s="2">
         <v>9557083</v>
@@ -1880,7 +2004,7 @@
       <c r="F40" s="2">
         <v>1</v>
       </c>
-      <c r="G40" s="2">
+      <c r="G40" s="3">
         <v>0.38200000000000001</v>
       </c>
       <c r="H40" s="3">
@@ -1890,24 +2014,24 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C41" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="F41" s="2">
         <v>5</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G41" s="3">
         <v>1.8</v>
       </c>
       <c r="H41" s="3">
@@ -1917,16 +2041,16 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E42" s="2">
         <v>1150164</v>
@@ -1934,7 +2058,7 @@
       <c r="F42" s="2">
         <v>1</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G42" s="3">
         <v>3.52</v>
       </c>
       <c r="H42" s="3">
@@ -1944,16 +2068,16 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="C43" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E43" s="2">
         <v>1053415</v>
@@ -1961,7 +2085,7 @@
       <c r="F43" s="2">
         <v>1</v>
       </c>
-      <c r="G43" s="2">
+      <c r="G43" s="3">
         <v>0.83599999999999997</v>
       </c>
       <c r="H43" s="3">
@@ -1969,28 +2093,738 @@
         <v>0.83599999999999997</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="14"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="11"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="12"/>
+    <row r="44" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A44" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+    </row>
+    <row r="45" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A45" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+    </row>
+    <row r="46" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A46" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+    </row>
+    <row r="47" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F48" s="2">
+        <v>100</v>
+      </c>
+      <c r="G48" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="H48" s="3">
+        <f>F48*G48</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="8">
+        <v>0</v>
+      </c>
+      <c r="G49" s="7">
+        <v>0</v>
+      </c>
+      <c r="H49" s="3">
+        <f t="shared" ref="H49:H60" si="3">F49*G49</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F50" s="2">
+        <v>10</v>
+      </c>
+      <c r="G50" s="3">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="H50" s="3">
+        <f t="shared" si="3"/>
+        <v>3.2800000000000002</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="8">
+        <v>0</v>
+      </c>
+      <c r="G51" s="7">
+        <v>0</v>
+      </c>
+      <c r="H51" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F52" s="2">
+        <v>5</v>
+      </c>
+      <c r="G52" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="H52" s="3">
+        <f t="shared" si="3"/>
+        <v>0.44999999999999996</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F53" s="2">
+        <v>5</v>
+      </c>
+      <c r="G53" s="3">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="H53" s="3">
+        <f t="shared" si="3"/>
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3">
+        <f>F54*G54</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E55" s="2">
+        <v>1146032</v>
+      </c>
+      <c r="F55" s="2">
+        <v>1</v>
+      </c>
+      <c r="G55" s="3">
+        <v>8.6</v>
+      </c>
+      <c r="H55" s="3">
+        <f>F55*G55</f>
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E56" s="2">
+        <v>2102513</v>
+      </c>
+      <c r="F56" s="2">
+        <v>1</v>
+      </c>
+      <c r="G56" s="3">
+        <v>5.17</v>
+      </c>
+      <c r="H56" s="3">
+        <f>F56*G56</f>
+        <v>5.17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E57" s="2">
+        <v>1507961</v>
+      </c>
+      <c r="F57" s="2">
+        <v>1</v>
+      </c>
+      <c r="G57" s="3">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="H57" s="3">
+        <f>F57*G57</f>
+        <v>0.57099999999999995</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3">
+        <f>F58*G58</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A59" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="12"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="12"/>
+    </row>
+    <row r="60" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A60" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B60" s="13"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+    </row>
+    <row r="61" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A61" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="14"/>
+    </row>
+    <row r="62" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="8">
+        <v>0</v>
+      </c>
+      <c r="G63" s="7">
+        <v>0</v>
+      </c>
+      <c r="H63" s="3">
+        <f>F63*G63</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E64" s="2">
+        <v>9724370</v>
+      </c>
+      <c r="F64" s="2">
+        <v>1</v>
+      </c>
+      <c r="G64" s="3">
+        <v>9.14</v>
+      </c>
+      <c r="H64" s="3">
+        <f t="shared" ref="H64:H83" si="4">F64*G64</f>
+        <v>9.14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C65" s="2">
+        <v>4832.232</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F65" s="2">
+        <v>2</v>
+      </c>
+      <c r="G65" s="3">
+        <v>5.48</v>
+      </c>
+      <c r="H65" s="3">
+        <f t="shared" si="4"/>
+        <v>10.96</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A67" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B67" s="12"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="12"/>
+    </row>
+    <row r="68" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A68" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B68" s="13"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+    </row>
+    <row r="69" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A69" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B69" s="14"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="14"/>
+    </row>
+    <row r="70" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="2"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="2"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="2"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="2"/>
+      <c r="B77" s="2"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="2"/>
+      <c r="B78" s="2"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="2"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="2"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="3"/>
+      <c r="H80" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="2"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="3"/>
+      <c r="H81" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="2"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="2"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="19">
+    <mergeCell ref="A67:H67"/>
+    <mergeCell ref="A68:H68"/>
+    <mergeCell ref="A69:H69"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="A59:H59"/>
+    <mergeCell ref="A60:H60"/>
+    <mergeCell ref="A61:H61"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="A44:H44"/>
+    <mergeCell ref="A45:H45"/>
+    <mergeCell ref="A46:H46"/>
+    <mergeCell ref="C49:E49"/>
     <mergeCell ref="C35:E35"/>
     <mergeCell ref="A22:H22"/>
     <mergeCell ref="A23:H23"/>
@@ -2001,8 +2835,11 @@
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape" r:id="rId1"/>
-  <rowBreaks count="1" manualBreakCount="1">
+  <rowBreaks count="4" manualBreakCount="4">
     <brk id="21" max="16383" man="1"/>
+    <brk id="43" max="16383" man="1"/>
+    <brk id="58" max="16383" man="1"/>
+    <brk id="66" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>